<commit_message>
updated BOM for 2022/23 batch
</commit_message>
<xml_diff>
--- a/Manufacturing/Rev A/BOM and CPL/SSTuino II BOM for Manufacturer - 20220703.xlsx
+++ b/Manufacturing/Rev A/BOM and CPL/SSTuino II BOM for Manufacturer - 20220703.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/panziyue/Documents/eagle/projects/SSTuino II/Manufacturing/Rev A/BOM and CPL/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07E7AC41-C52C-9143-BFE9-D55212DB0412}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B12674B-2931-EF4A-83CA-0B3174726B04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM" sheetId="1" r:id="rId1"/>
@@ -499,7 +499,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="dd/mm/yyyy;@"/>
+    <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
   </numFmts>
   <fonts count="12" x14ac:knownFonts="1">
     <font>
@@ -580,7 +580,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -596,6 +596,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -647,7 +653,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -696,10 +702,12 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1043,8 +1051,8 @@
   </sheetPr>
   <dimension ref="A1:M41"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="109" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="I31" sqref="I31"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A10" zoomScale="109" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -1624,16 +1632,16 @@
       <c r="A25" s="14">
         <v>14</v>
       </c>
-      <c r="B25" s="20" t="s">
+      <c r="B25" s="28" t="s">
         <v>78</v>
       </c>
-      <c r="C25" s="20" t="s">
+      <c r="C25" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="D25" s="15" t="s">
+      <c r="D25" s="29" t="s">
         <v>53</v>
       </c>
-      <c r="E25" s="15" t="s">
+      <c r="E25" s="29" t="s">
         <v>113</v>
       </c>
       <c r="F25" s="17" t="s">
@@ -1792,16 +1800,16 @@
       <c r="A30" s="14">
         <v>19</v>
       </c>
-      <c r="B30" s="20" t="s">
+      <c r="B30" s="28" t="s">
         <v>83</v>
       </c>
-      <c r="C30" s="20" t="s">
+      <c r="C30" s="28" t="s">
         <v>40</v>
       </c>
-      <c r="D30" s="15" t="s">
+      <c r="D30" s="29" t="s">
         <v>57</v>
       </c>
-      <c r="E30" s="15" t="s">
+      <c r="E30" s="29" t="s">
         <v>113</v>
       </c>
       <c r="F30" s="17"/>
@@ -1822,16 +1830,16 @@
       <c r="A31" s="14">
         <v>20</v>
       </c>
-      <c r="B31" s="20" t="s">
+      <c r="B31" s="28" t="s">
         <v>84</v>
       </c>
-      <c r="C31" s="20" t="s">
+      <c r="C31" s="28" t="s">
         <v>146</v>
       </c>
-      <c r="D31" s="15" t="s">
+      <c r="D31" s="29" t="s">
         <v>58</v>
       </c>
-      <c r="E31" s="15" t="s">
+      <c r="E31" s="29" t="s">
         <v>113</v>
       </c>
       <c r="F31" s="17" t="s">
@@ -1890,16 +1898,16 @@
       <c r="A33" s="14">
         <v>22</v>
       </c>
-      <c r="B33" s="20" t="s">
+      <c r="B33" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="C33" s="20" t="s">
+      <c r="C33" s="28" t="s">
         <v>42</v>
       </c>
-      <c r="D33" s="15" t="s">
+      <c r="D33" s="29" t="s">
         <v>42</v>
       </c>
-      <c r="E33" s="15" t="s">
+      <c r="E33" s="29" t="s">
         <v>113</v>
       </c>
       <c r="F33" s="17" t="s">
@@ -1922,16 +1930,16 @@
       <c r="A34" s="14">
         <v>23</v>
       </c>
-      <c r="B34" s="20" t="s">
+      <c r="B34" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="C34" s="20" t="s">
+      <c r="C34" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="D34" s="15" t="s">
+      <c r="D34" s="29" t="s">
         <v>60</v>
       </c>
-      <c r="E34" s="15" t="s">
+      <c r="E34" s="29" t="s">
         <v>113</v>
       </c>
       <c r="F34" s="17"/>
@@ -2080,16 +2088,16 @@
       <c r="A39" s="14">
         <v>28</v>
       </c>
-      <c r="B39" s="20" t="s">
+      <c r="B39" s="28" t="s">
         <v>135</v>
       </c>
-      <c r="C39" s="20" t="s">
+      <c r="C39" s="28" t="s">
         <v>137</v>
       </c>
-      <c r="D39" s="15" t="s">
+      <c r="D39" s="29" t="s">
         <v>136</v>
       </c>
-      <c r="E39" s="15" t="s">
+      <c r="E39" s="29" t="s">
         <v>145</v>
       </c>
       <c r="F39" s="17"/>

</xml_diff>